<commit_message>
Deleted My Account - My Profile
</commit_message>
<xml_diff>
--- a/MabTest11/Test/Main.rvl.xlsx
+++ b/MabTest11/Test/Main.rvl.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="27">
   <si>
     <t>Flow</t>
   </si>
@@ -88,6 +88,12 @@
   </si>
   <si>
     <t>dnn$ctr504$BasicInformation$ctl0</t>
+  </si>
+  <si>
+    <t>Click on Save</t>
+  </si>
+  <si>
+    <t>Save</t>
   </si>
 </sst>
 </file>
@@ -108,7 +114,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="172">
+  <borders count="174">
     <border>
       <left/>
       <right/>
@@ -287,11 +293,13 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="172">
+  <cellXfs count="174">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0"/>
@@ -464,6 +472,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="169" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="170" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="171" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="172" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="173" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -473,7 +483,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H23"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.7109375" customWidth="true"/>
@@ -513,84 +523,83 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="16"/>
+      <c r="A2" s="161" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="161" t="s">
+      <c r="A3" s="165" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="G3" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="162" t="s">
-        <v>8</v>
+      <c r="A4" s="169" t="s">
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="G4" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="163" t="s">
+      <c r="A5" s="171" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
@@ -606,368 +615,184 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="164" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" t="s">
-        <v>7</v>
-      </c>
+      <c r="A6" s="17"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="24"/>
     </row>
     <row r="7">
-      <c r="A7" s="165" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" t="s">
-        <v>18</v>
-      </c>
+      <c r="A7" s="25"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="32"/>
     </row>
     <row r="8">
-      <c r="A8" s="166" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8" t="s">
-        <v>7</v>
-      </c>
+      <c r="A8" s="33"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="40"/>
     </row>
     <row r="9">
-      <c r="A9" s="167" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" t="s">
-        <v>7</v>
-      </c>
-      <c r="G9" t="s">
-        <v>7</v>
-      </c>
+      <c r="A9" s="41"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="48"/>
     </row>
     <row r="10">
-      <c r="A10" s="168" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" t="s">
-        <v>7</v>
-      </c>
-      <c r="G10" t="s">
-        <v>7</v>
-      </c>
+      <c r="A10" s="49"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="54"/>
+      <c r="G10" s="55"/>
+      <c r="H10" s="56"/>
     </row>
     <row r="11">
-      <c r="A11" s="169" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" t="s">
-        <v>22</v>
-      </c>
+      <c r="A11" s="57"/>
+      <c r="B11" s="58"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="61"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="63"/>
+      <c r="H11" s="64"/>
     </row>
     <row r="12">
-      <c r="A12" s="170" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" t="s">
-        <v>7</v>
-      </c>
-      <c r="F12" t="s">
-        <v>7</v>
-      </c>
-      <c r="G12" t="s">
-        <v>7</v>
-      </c>
+      <c r="A12" s="65"/>
+      <c r="B12" s="66"/>
+      <c r="C12" s="67"/>
+      <c r="D12" s="68"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="70"/>
+      <c r="G12" s="71"/>
+      <c r="H12" s="72"/>
     </row>
     <row r="13">
-      <c r="A13" s="171" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" t="s">
-        <v>7</v>
-      </c>
-      <c r="G13" t="s">
-        <v>7</v>
-      </c>
+      <c r="A13" s="73"/>
+      <c r="B13" s="74"/>
+      <c r="C13" s="75"/>
+      <c r="D13" s="76"/>
+      <c r="E13" s="77"/>
+      <c r="F13" s="78"/>
+      <c r="G13" s="79"/>
+      <c r="H13" s="80"/>
     </row>
     <row r="14">
-      <c r="A14" s="17"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="24"/>
+      <c r="A14" s="81"/>
+      <c r="B14" s="82"/>
+      <c r="C14" s="83"/>
+      <c r="D14" s="84"/>
+      <c r="E14" s="85"/>
+      <c r="F14" s="86"/>
+      <c r="G14" s="87"/>
+      <c r="H14" s="88"/>
     </row>
     <row r="15">
-      <c r="A15" s="25"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="32"/>
+      <c r="A15" s="89"/>
+      <c r="B15" s="90"/>
+      <c r="C15" s="91"/>
+      <c r="D15" s="92"/>
+      <c r="E15" s="93"/>
+      <c r="F15" s="94"/>
+      <c r="G15" s="95"/>
+      <c r="H15" s="96"/>
     </row>
     <row r="16">
-      <c r="A16" s="33"/>
-      <c r="B16" s="34"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="40"/>
+      <c r="A16" s="97"/>
+      <c r="B16" s="98"/>
+      <c r="C16" s="99"/>
+      <c r="D16" s="100"/>
+      <c r="E16" s="101"/>
+      <c r="F16" s="102"/>
+      <c r="G16" s="103"/>
+      <c r="H16" s="104"/>
     </row>
     <row r="17">
-      <c r="A17" s="41"/>
-      <c r="B17" s="42"/>
-      <c r="C17" s="43"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="48"/>
+      <c r="A17" s="105"/>
+      <c r="B17" s="106"/>
+      <c r="C17" s="107"/>
+      <c r="D17" s="108"/>
+      <c r="E17" s="109"/>
+      <c r="F17" s="110"/>
+      <c r="G17" s="111"/>
+      <c r="H17" s="112"/>
     </row>
     <row r="18">
-      <c r="A18" s="49"/>
-      <c r="B18" s="50"/>
-      <c r="C18" s="51"/>
-      <c r="D18" s="52"/>
-      <c r="E18" s="53"/>
-      <c r="F18" s="54"/>
-      <c r="G18" s="55"/>
-      <c r="H18" s="56"/>
+      <c r="A18" s="113"/>
+      <c r="B18" s="114"/>
+      <c r="C18" s="115"/>
+      <c r="D18" s="116"/>
+      <c r="E18" s="117"/>
+      <c r="F18" s="118"/>
+      <c r="G18" s="119"/>
+      <c r="H18" s="120"/>
     </row>
     <row r="19">
-      <c r="A19" s="57"/>
-      <c r="B19" s="58"/>
-      <c r="C19" s="59"/>
-      <c r="D19" s="60"/>
-      <c r="E19" s="61"/>
-      <c r="F19" s="62"/>
-      <c r="G19" s="63"/>
-      <c r="H19" s="64"/>
+      <c r="A19" s="121"/>
+      <c r="B19" s="122"/>
+      <c r="C19" s="123"/>
+      <c r="D19" s="124"/>
+      <c r="E19" s="125"/>
+      <c r="F19" s="126"/>
+      <c r="G19" s="127"/>
+      <c r="H19" s="128"/>
     </row>
     <row r="20">
-      <c r="A20" s="65"/>
-      <c r="B20" s="66"/>
-      <c r="C20" s="67"/>
-      <c r="D20" s="68"/>
-      <c r="E20" s="69"/>
-      <c r="F20" s="70"/>
-      <c r="G20" s="71"/>
-      <c r="H20" s="72"/>
+      <c r="A20" s="129"/>
+      <c r="B20" s="130"/>
+      <c r="C20" s="131"/>
+      <c r="D20" s="132"/>
+      <c r="E20" s="133"/>
+      <c r="F20" s="134"/>
+      <c r="G20" s="135"/>
+      <c r="H20" s="136"/>
     </row>
     <row r="21">
-      <c r="A21" s="73"/>
-      <c r="B21" s="74"/>
-      <c r="C21" s="75"/>
-      <c r="D21" s="76"/>
-      <c r="E21" s="77"/>
-      <c r="F21" s="78"/>
-      <c r="G21" s="79"/>
-      <c r="H21" s="80"/>
+      <c r="A21" s="137"/>
+      <c r="B21" s="138"/>
+      <c r="C21" s="139"/>
+      <c r="D21" s="140"/>
+      <c r="E21" s="141"/>
+      <c r="F21" s="142"/>
+      <c r="G21" s="143"/>
+      <c r="H21" s="144"/>
     </row>
     <row r="22">
-      <c r="A22" s="81"/>
-      <c r="B22" s="82"/>
-      <c r="C22" s="83"/>
-      <c r="D22" s="84"/>
-      <c r="E22" s="85"/>
-      <c r="F22" s="86"/>
-      <c r="G22" s="87"/>
-      <c r="H22" s="88"/>
+      <c r="A22" s="145"/>
+      <c r="B22" s="146"/>
+      <c r="C22" s="147"/>
+      <c r="D22" s="148"/>
+      <c r="E22" s="149"/>
+      <c r="F22" s="150"/>
+      <c r="G22" s="151"/>
+      <c r="H22" s="152"/>
     </row>
     <row r="23">
-      <c r="A23" s="89"/>
-      <c r="B23" s="90"/>
-      <c r="C23" s="91"/>
-      <c r="D23" s="92"/>
-      <c r="E23" s="93"/>
-      <c r="F23" s="94"/>
-      <c r="G23" s="95"/>
-      <c r="H23" s="96"/>
-    </row>
-    <row r="24">
-      <c r="A24" s="97"/>
-      <c r="B24" s="98"/>
-      <c r="C24" s="99"/>
-      <c r="D24" s="100"/>
-      <c r="E24" s="101"/>
-      <c r="F24" s="102"/>
-      <c r="G24" s="103"/>
-      <c r="H24" s="104"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="105"/>
-      <c r="B25" s="106"/>
-      <c r="C25" s="107"/>
-      <c r="D25" s="108"/>
-      <c r="E25" s="109"/>
-      <c r="F25" s="110"/>
-      <c r="G25" s="111"/>
-      <c r="H25" s="112"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="113"/>
-      <c r="B26" s="114"/>
-      <c r="C26" s="115"/>
-      <c r="D26" s="116"/>
-      <c r="E26" s="117"/>
-      <c r="F26" s="118"/>
-      <c r="G26" s="119"/>
-      <c r="H26" s="120"/>
-    </row>
-    <row r="27">
-      <c r="A27" s="121"/>
-      <c r="B27" s="122"/>
-      <c r="C27" s="123"/>
-      <c r="D27" s="124"/>
-      <c r="E27" s="125"/>
-      <c r="F27" s="126"/>
-      <c r="G27" s="127"/>
-      <c r="H27" s="128"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="129"/>
-      <c r="B28" s="130"/>
-      <c r="C28" s="131"/>
-      <c r="D28" s="132"/>
-      <c r="E28" s="133"/>
-      <c r="F28" s="134"/>
-      <c r="G28" s="135"/>
-      <c r="H28" s="136"/>
-    </row>
-    <row r="29">
-      <c r="A29" s="137"/>
-      <c r="B29" s="138"/>
-      <c r="C29" s="139"/>
-      <c r="D29" s="140"/>
-      <c r="E29" s="141"/>
-      <c r="F29" s="142"/>
-      <c r="G29" s="143"/>
-      <c r="H29" s="144"/>
-    </row>
-    <row r="30">
-      <c r="A30" s="145"/>
-      <c r="B30" s="146"/>
-      <c r="C30" s="147"/>
-      <c r="D30" s="148"/>
-      <c r="E30" s="149"/>
-      <c r="F30" s="150"/>
-      <c r="G30" s="151"/>
-      <c r="H30" s="152"/>
-    </row>
-    <row r="31">
-      <c r="A31" s="153"/>
-      <c r="B31" s="154"/>
-      <c r="C31" s="155"/>
-      <c r="D31" s="156"/>
-      <c r="E31" s="157"/>
-      <c r="F31" s="158"/>
-      <c r="G31" s="159"/>
-      <c r="H31" s="160"/>
+      <c r="A23" s="153"/>
+      <c r="B23" s="154"/>
+      <c r="C23" s="155"/>
+      <c r="D23" s="156"/>
+      <c r="E23" s="157"/>
+      <c r="F23" s="158"/>
+      <c r="G23" s="159"/>
+      <c r="H23" s="160"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>